<commit_message>
Update Product-Backlog 3 and Sprint-Backlog 3
</commit_message>
<xml_diff>
--- a/Product-Backlog.xlsx
+++ b/Product-Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -101,19 +101,13 @@
     <t>Column1</t>
   </si>
   <si>
-    <t>Up video lên các mạng xã hội</t>
-  </si>
-  <si>
-    <t>Giúp giới thiệu về bản thân</t>
-  </si>
-  <si>
-    <t>Up được video lên các mạng xã hội</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thấy được những điều cần lưu ý (nội dung, background, nhạc, công cụ, …) khi làm một video </t>
   </si>
   <si>
     <t>Dễ gây ấn tượng cho người xem hơn.</t>
+  </si>
+  <si>
+    <t>finished</t>
   </si>
 </sst>
 </file>
@@ -296,6 +290,12 @@
   <dxfs count="14">
     <dxf>
       <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -703,12 +703,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -723,23 +717,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:K6"/>
   <sortState ref="A2:K6">
     <sortCondition descending="1" ref="J1:J6"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" name="ID" dataDxfId="10"/>
-    <tableColumn id="3" name="As a / an" dataDxfId="9"/>
-    <tableColumn id="4" name="I want to…" dataDxfId="8"/>
-    <tableColumn id="5" name="so that…" dataDxfId="7"/>
-    <tableColumn id="6" name="notes" dataDxfId="6"/>
-    <tableColumn id="9" name="acceptance criteria" dataDxfId="5"/>
-    <tableColumn id="7" name="added in sprint" dataDxfId="4"/>
-    <tableColumn id="2" name="estimated time" dataDxfId="3"/>
-    <tableColumn id="10" name="remaining time" dataDxfId="2"/>
-    <tableColumn id="8" name="priority" dataDxfId="1"/>
-    <tableColumn id="11" name="Column1" dataDxfId="0">
+    <tableColumn id="1" name="ID" dataDxfId="11"/>
+    <tableColumn id="3" name="As a / an" dataDxfId="10"/>
+    <tableColumn id="4" name="I want to…" dataDxfId="9"/>
+    <tableColumn id="5" name="so that…" dataDxfId="8"/>
+    <tableColumn id="6" name="notes" dataDxfId="7"/>
+    <tableColumn id="9" name="acceptance criteria" dataDxfId="6"/>
+    <tableColumn id="7" name="added in sprint" dataDxfId="5"/>
+    <tableColumn id="2" name="estimated time" dataDxfId="4"/>
+    <tableColumn id="10" name="remaining time" dataDxfId="3"/>
+    <tableColumn id="8" name="priority" dataDxfId="2"/>
+    <tableColumn id="11" name="Column1" dataDxfId="1">
       <calculatedColumnFormula>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1010,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1073,23 +1067,23 @@
         <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="G2" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" s="12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I2" s="12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J2" s="6">
         <v>60</v>
@@ -1101,37 +1095,37 @@
       <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
-        <v>4</v>
+      <c r="A3" s="6">
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="11">
-        <v>2</v>
-      </c>
-      <c r="H3" s="6">
-        <v>5</v>
-      </c>
-      <c r="I3" s="6">
-        <v>5</v>
-      </c>
-      <c r="J3" s="9">
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="8">
+        <v>3</v>
+      </c>
+      <c r="H3" s="8">
+        <v>3</v>
+      </c>
+      <c r="I3" s="8">
+        <v>3</v>
+      </c>
+      <c r="J3" s="6">
         <v>50</v>
       </c>
       <c r="K3" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Giới thiệu cách tạo video từ một công cụ so that Có thể tự mình làm được video để đi phỏng vấn.</v>
+        <v>As a / an website visitor I want to Thấy công dụng việc làm video. so that Biết lợi ích khi có một video giới thiệu về cá nhân.</v>
       </c>
       <c r="L3" s="16"/>
     </row>
@@ -1152,7 +1146,9 @@
       <c r="F4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="11">
+        <v>4</v>
+      </c>
       <c r="H4" s="6">
         <v>5</v>
       </c>
@@ -1173,35 +1169,37 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>2</v>
+      <c r="A5" s="9">
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
-        <v>2</v>
-      </c>
-      <c r="I5" s="8">
-        <v>2</v>
-      </c>
-      <c r="J5" s="6">
-        <v>30</v>
+      <c r="C5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0</v>
       </c>
       <c r="K5" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Thấy công dụng việc làm video. so that Biết lợi ích khi có một video giới thiệu về cá nhân.</v>
+        <v>As a / an website visitor I want to Giới thiệu cách tạo video từ một công cụ so that Có thể tự mình làm được video để đi phỏng vấn.</v>
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="4"/>
@@ -1226,15 +1224,17 @@
       <c r="F6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="H6" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K6" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
@@ -1246,41 +1246,9 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="6">
-        <v>2</v>
-      </c>
-      <c r="I7" s="6">
-        <v>2</v>
-      </c>
-      <c r="J7" s="9">
-        <v>10</v>
-      </c>
-      <c r="K7" s="11" t="str">
-        <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Up video lên các mạng xã hội so that Giúp giới thiệu về bản thân</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:I1048576">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!="rejected"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update Product + Sprint Backlog
</commit_message>
<xml_diff>
--- a/Product-Backlog.xlsx
+++ b/Product-Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>finished</t>
+  </si>
+  <si>
+    <t>Có poster</t>
+  </si>
+  <si>
+    <t>giới thiệu sản phẩm</t>
+  </si>
+  <si>
+    <t>Poster đầy đủ nội dung</t>
+  </si>
+  <si>
+    <t>visitor</t>
   </si>
 </sst>
 </file>
@@ -230,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -282,12 +294,87 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -717,23 +804,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:K6"/>
-  <sortState ref="A2:K6">
-    <sortCondition descending="1" ref="J1:J6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K7" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:K7"/>
+  <sortState ref="A2:K7">
+    <sortCondition descending="1" ref="J1:J7"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" name="ID" dataDxfId="11"/>
-    <tableColumn id="3" name="As a / an" dataDxfId="10"/>
-    <tableColumn id="4" name="I want to…" dataDxfId="9"/>
-    <tableColumn id="5" name="so that…" dataDxfId="8"/>
-    <tableColumn id="6" name="notes" dataDxfId="7"/>
-    <tableColumn id="9" name="acceptance criteria" dataDxfId="6"/>
-    <tableColumn id="7" name="added in sprint" dataDxfId="5"/>
-    <tableColumn id="2" name="estimated time" dataDxfId="4"/>
-    <tableColumn id="10" name="remaining time" dataDxfId="3"/>
-    <tableColumn id="8" name="priority" dataDxfId="2"/>
-    <tableColumn id="11" name="Column1" dataDxfId="1">
+    <tableColumn id="1" name="ID" dataDxfId="23"/>
+    <tableColumn id="3" name="As a / an" dataDxfId="22"/>
+    <tableColumn id="4" name="I want to…" dataDxfId="21"/>
+    <tableColumn id="5" name="so that…" dataDxfId="20"/>
+    <tableColumn id="6" name="notes" dataDxfId="19"/>
+    <tableColumn id="9" name="acceptance criteria" dataDxfId="18"/>
+    <tableColumn id="7" name="added in sprint" dataDxfId="17"/>
+    <tableColumn id="2" name="estimated time" dataDxfId="16"/>
+    <tableColumn id="10" name="remaining time" dataDxfId="15"/>
+    <tableColumn id="8" name="priority" dataDxfId="14"/>
+    <tableColumn id="11" name="Column1" dataDxfId="13">
       <calculatedColumnFormula>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1004,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1060,107 +1147,107 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>3</v>
+      <c r="A2" s="9">
+        <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="12">
-        <v>3</v>
-      </c>
-      <c r="H2" s="12">
-        <v>3</v>
-      </c>
-      <c r="I2" s="12">
-        <v>3</v>
-      </c>
-      <c r="J2" s="6">
-        <v>60</v>
+      <c r="C2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="11">
+        <v>4</v>
+      </c>
+      <c r="H2" s="6">
+        <v>5</v>
+      </c>
+      <c r="I2" s="6">
+        <v>5</v>
+      </c>
+      <c r="J2" s="9">
+        <v>40</v>
       </c>
       <c r="K2" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Thấy được những điều cần lưu ý (nội dung, background, nhạc, công cụ, …) khi làm một video  so that Dễ gây ấn tượng cho người xem hơn.</v>
+        <v>As a / an website visitor I want to Thấy được một video hướng dẫn và một số video của những người đã làm so that Thấy hướng dẫn chi tiết và sản phẩm tiêu biểu.</v>
       </c>
       <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>2</v>
+      <c r="A3" s="9">
+        <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="8">
-        <v>3</v>
-      </c>
-      <c r="H3" s="8">
-        <v>3</v>
-      </c>
-      <c r="I3" s="8">
-        <v>3</v>
-      </c>
-      <c r="J3" s="6">
-        <v>50</v>
+        <v>31</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="11">
+        <v>4</v>
+      </c>
+      <c r="H3" s="6">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6">
+        <v>5</v>
+      </c>
+      <c r="J3" s="9">
+        <v>40</v>
       </c>
       <c r="K3" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Thấy công dụng việc làm video. so that Biết lợi ích khi có một video giới thiệu về cá nhân.</v>
+        <v>As a / an visitor I want to Có poster so that giới thiệu sản phẩm</v>
       </c>
       <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
-        <v>5</v>
+      <c r="A4" s="6">
+        <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="11">
-        <v>4</v>
-      </c>
-      <c r="H4" s="6">
-        <v>5</v>
-      </c>
-      <c r="I4" s="6">
-        <v>5</v>
-      </c>
-      <c r="J4" s="9">
-        <v>40</v>
+      <c r="C4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="12">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12">
+        <v>3</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
       </c>
       <c r="K4" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Thấy được một video hướng dẫn và một số video của những người đã làm so that Thấy hướng dẫn chi tiết và sản phẩm tiêu biểu.</v>
+        <v>As a / an website visitor I want to Thấy được những điều cần lưu ý (nội dung, background, nhạc, công cụ, …) khi làm một video  so that Dễ gây ấn tượng cho người xem hơn.</v>
       </c>
       <c r="L4" s="16"/>
       <c r="M4" s="5"/>
@@ -1169,37 +1256,37 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
-        <v>4</v>
+      <c r="A5" s="6">
+        <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="9">
+      <c r="H5" s="8">
+        <v>3</v>
+      </c>
+      <c r="I5" s="8">
+        <v>3</v>
+      </c>
+      <c r="J5" s="6">
         <v>0</v>
       </c>
       <c r="K5" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Giới thiệu cách tạo video từ một công cụ so that Có thể tự mình làm được video để đi phỏng vấn.</v>
+        <v>As a / an website visitor I want to Thấy công dụng việc làm video. so that Biết lợi ích khi có một video giới thiệu về cá nhân.</v>
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="4"/>
@@ -1208,37 +1295,37 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>1</v>
+      <c r="A6" s="9">
+        <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="6">
         <v>0</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="6">
         <v>0</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="9">
         <v>0</v>
       </c>
       <c r="K6" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Thấy được bố cục của trang web (trang chủ) so that Hiểu trang web hơn</v>
+        <v>As a / an website visitor I want to Giới thiệu cách tạo video từ một công cụ so that Có thể tự mình làm được video để đi phỏng vấn.</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="4"/>
@@ -1246,8 +1333,58 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
+    <row r="7" spans="1:16" s="4" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
+      <c r="K7" s="14" t="str">
+        <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
+        <v>As a / an website visitor I want to Thấy được bố cục của trang web (trang chủ) so that Hiểu trang web hơn</v>
+      </c>
+      <c r="L7" s="16"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:I1048576">
+  <conditionalFormatting sqref="A8:I1048576 A1:I6 E7">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>#REF!="rejected"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:D7 F7:I7">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>#REF!="rejected"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>#REF!="rejected"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!="rejected"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update Product-Backlog and Sprint-Backlog
</commit_message>
<xml_diff>
--- a/Product-Backlog.xlsx
+++ b/Product-Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TonThat\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\NMCNTT2-PROJECT1.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -302,73 +302,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <font>
         <strike/>
@@ -789,6 +723,30 @@
           <color indexed="64"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -804,23 +762,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K7" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:K7"/>
   <sortState ref="A2:K7">
-    <sortCondition descending="1" ref="J1:J7"/>
+    <sortCondition ref="A1:A7"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" name="ID" dataDxfId="23"/>
-    <tableColumn id="3" name="As a / an" dataDxfId="22"/>
-    <tableColumn id="4" name="I want to…" dataDxfId="21"/>
-    <tableColumn id="5" name="so that…" dataDxfId="20"/>
-    <tableColumn id="6" name="notes" dataDxfId="19"/>
-    <tableColumn id="9" name="acceptance criteria" dataDxfId="18"/>
-    <tableColumn id="7" name="added in sprint" dataDxfId="17"/>
-    <tableColumn id="2" name="estimated time" dataDxfId="16"/>
-    <tableColumn id="10" name="remaining time" dataDxfId="15"/>
-    <tableColumn id="8" name="priority" dataDxfId="14"/>
-    <tableColumn id="11" name="Column1" dataDxfId="13">
+    <tableColumn id="1" name="ID" dataDxfId="12"/>
+    <tableColumn id="3" name="As a / an" dataDxfId="11"/>
+    <tableColumn id="4" name="I want to…" dataDxfId="10"/>
+    <tableColumn id="5" name="so that…" dataDxfId="9"/>
+    <tableColumn id="6" name="notes" dataDxfId="8"/>
+    <tableColumn id="9" name="acceptance criteria" dataDxfId="7"/>
+    <tableColumn id="7" name="added in sprint" dataDxfId="6"/>
+    <tableColumn id="2" name="estimated time" dataDxfId="5"/>
+    <tableColumn id="10" name="remaining time" dataDxfId="4"/>
+    <tableColumn id="8" name="priority" dataDxfId="3"/>
+    <tableColumn id="11" name="Column1" dataDxfId="2">
       <calculatedColumnFormula>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1094,7 +1052,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1147,72 +1105,72 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
-        <v>5</v>
+      <c r="A2" s="6">
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="11">
-        <v>4</v>
-      </c>
-      <c r="H2" s="6">
-        <v>5</v>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0</v>
       </c>
       <c r="I2" s="6">
-        <v>5</v>
-      </c>
-      <c r="J2" s="9">
-        <v>40</v>
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
       </c>
       <c r="K2" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Thấy được một video hướng dẫn và một số video của những người đã làm so that Thấy hướng dẫn chi tiết và sản phẩm tiêu biểu.</v>
+        <v>As a / an website visitor I want to Thấy được bố cục của trang web (trang chủ) so that Hiểu trang web hơn</v>
       </c>
       <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
-        <v>6</v>
+      <c r="A3" s="6">
+        <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="11">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="H3" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I3" s="6">
-        <v>5</v>
-      </c>
-      <c r="J3" s="9">
-        <v>40</v>
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
       </c>
       <c r="K3" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an visitor I want to Có poster so that giới thiệu sản phẩm</v>
+        <v>As a / an website visitor I want to Thấy công dụng việc làm video. so that Biết lợi ích khi có một video giới thiệu về cá nhân.</v>
       </c>
       <c r="L3" s="16"/>
     </row>
@@ -1236,11 +1194,11 @@
       <c r="G4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="12">
-        <v>3</v>
-      </c>
-      <c r="I4" s="12">
-        <v>3</v>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
       </c>
       <c r="J4" s="6">
         <v>0</v>
@@ -1256,37 +1214,37 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>2</v>
+      <c r="A5" s="9">
+        <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="C5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="8">
-        <v>3</v>
-      </c>
-      <c r="I5" s="8">
-        <v>3</v>
-      </c>
-      <c r="J5" s="6">
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9">
         <v>0</v>
       </c>
       <c r="K5" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Thấy công dụng việc làm video. so that Biết lợi ích khi có một video giới thiệu về cá nhân.</v>
+        <v>As a / an website visitor I want to Giới thiệu cách tạo video từ một công cụ so that Có thể tự mình làm được video để đi phỏng vấn.</v>
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="4"/>
@@ -1296,20 +1254,20 @@
     </row>
     <row r="6" spans="1:16" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>27</v>
@@ -1325,7 +1283,7 @@
       </c>
       <c r="K6" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Giới thiệu cách tạo video từ một công cụ so that Có thể tự mình làm được video để đi phỏng vấn.</v>
+        <v>As a / an website visitor I want to Thấy được một video hướng dẫn và một số video của những người đã làm so that Thấy hướng dẫn chi tiết và sản phẩm tiêu biểu.</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="4"/>
@@ -1334,58 +1292,58 @@
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16" s="4" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>1</v>
+      <c r="A7" s="9">
+        <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" s="9">
         <v>0</v>
       </c>
       <c r="K7" s="14" t="str">
         <f>"As a / an " &amp; Table1[[#This Row],[As a / an]] &amp; " I want to " &amp; Table1[[#This Row],[I want to…]] &amp; " so that " &amp; Table1[[#This Row],[so that…]]</f>
-        <v>As a / an website visitor I want to Thấy được bố cục của trang web (trang chủ) so that Hiểu trang web hơn</v>
+        <v>As a / an visitor I want to Có poster so that giới thiệu sản phẩm</v>
       </c>
       <c r="L7" s="16"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A8:I1048576 A1:I6 E7">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="A8:I1048576 A1:I2 E7 I3:I7 A3:H6">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>#REF!="rejected"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:D7 F7:I7">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="C7:D7 F7:H7">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>#REF!="rejected"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>#REF!="rejected"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>#REF!="rejected"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>